<commit_message>
completed facilities document.  added current and pending, and completed first draft of budget justification
</commit_message>
<xml_diff>
--- a/NSF_Career_Budget_Hanson3.xlsx
+++ b/NSF_Career_Budget_Hanson3.xlsx
@@ -679,7 +679,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="120">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1023,42 +1023,6 @@
     <xf numFmtId="174" fontId="4" fillId="5" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="4" fillId="0" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="175" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="175" fontId="4" fillId="6" borderId="3" xfId="15" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -1276,8 +1240,8 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1540,16 +1504,16 @@
         <v>16771.248</v>
       </c>
       <c r="H11" s="43" t="n">
-        <f aca="false">G11*1.02</f>
-        <v>17106.67296</v>
+        <f aca="false">G11*1.02*2/4</f>
+        <v>8553.33648</v>
       </c>
       <c r="I11" s="43" t="n">
-        <f aca="false">H11*1.02</f>
+        <f aca="false">H11*1.02*4/2</f>
         <v>17448.8064192</v>
       </c>
       <c r="J11" s="43" t="n">
         <f aca="false">SUM(E11:I11)</f>
-        <v>87999.7273792</v>
+        <v>79446.3908992</v>
       </c>
     </row>
     <row r="12" s="26" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,24 +1535,24 @@
         <v>8370</v>
       </c>
       <c r="F12" s="43" t="n">
-        <f aca="false">E12*1.02*0.33</f>
-        <v>2817.342</v>
+        <f aca="false">E12*1.02*1/3</f>
+        <v>2845.8</v>
       </c>
       <c r="G12" s="43" t="n">
         <f aca="false">F12*1.02*3</f>
-        <v>8621.06652</v>
+        <v>8708.148</v>
       </c>
       <c r="H12" s="43" t="n">
-        <f aca="false">G12*1.02*0.33</f>
-        <v>2901.850990632</v>
+        <f aca="false">G12*1.02*2/3</f>
+        <v>5921.54064</v>
       </c>
       <c r="I12" s="43" t="n">
         <f aca="false">H12*1.02</f>
-        <v>2959.88801044464</v>
+        <v>6039.9714528</v>
       </c>
       <c r="J12" s="43" t="n">
         <f aca="false">SUM(E12:I12)</f>
-        <v>25670.1475210766</v>
+        <v>31885.4600928</v>
       </c>
     </row>
     <row r="13" s="26" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,35 +1563,35 @@
         <v>25</v>
       </c>
       <c r="C13" s="42" t="n">
-        <f aca="false">19*10</f>
-        <v>190</v>
+        <f aca="false">18*10</f>
+        <v>180</v>
       </c>
       <c r="D13" s="30" t="n">
         <v>2</v>
       </c>
       <c r="E13" s="35" t="n">
         <f aca="false">B13*C13*D13</f>
-        <v>9500</v>
+        <v>9000</v>
       </c>
       <c r="F13" s="35" t="n">
         <f aca="false">E13*1.02</f>
-        <v>9690</v>
+        <v>9180</v>
       </c>
       <c r="G13" s="35" t="n">
         <f aca="false">F13*1.02</f>
-        <v>9883.8</v>
+        <v>9363.6</v>
       </c>
       <c r="H13" s="35" t="n">
         <f aca="false">G13*1.02</f>
-        <v>10081.476</v>
+        <v>9550.872</v>
       </c>
       <c r="I13" s="35" t="n">
         <f aca="false">H13*1.02</f>
-        <v>10283.10552</v>
+        <v>9741.88944</v>
       </c>
       <c r="J13" s="35" t="n">
         <f aca="false">SUM(E13:I13)</f>
-        <v>49438.38152</v>
+        <v>46836.36144</v>
       </c>
     </row>
     <row r="14" s="26" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,27 +1633,27 @@
       <c r="D15" s="47"/>
       <c r="E15" s="48" t="n">
         <f aca="false">SUM(E8:E14)</f>
-        <v>49730.64</v>
+        <v>49230.64</v>
       </c>
       <c r="F15" s="48" t="n">
         <f aca="false">SUM(F8:F14)</f>
-        <v>49115.7948</v>
+        <v>48634.2528</v>
       </c>
       <c r="G15" s="48" t="n">
         <f aca="false">SUM(G8:G14)</f>
-        <v>51652.676376</v>
+        <v>51219.557856</v>
       </c>
       <c r="H15" s="48" t="n">
         <f aca="false">SUM(H8:H14)</f>
-        <v>46794.093043752</v>
+        <v>40729.84221312</v>
       </c>
       <c r="I15" s="48" t="n">
         <f aca="false">SUM(I8:I14)</f>
-        <v>47729.974904627</v>
+        <v>50268.8422669824</v>
       </c>
       <c r="J15" s="48" t="n">
         <f aca="false">SUM(J8:J14)</f>
-        <v>245023.179124379</v>
+        <v>240083.135136102</v>
       </c>
       <c r="K15" s="49"/>
       <c r="L15" s="49"/>
@@ -1793,7 +1757,7 @@
       </c>
       <c r="H19" s="35" t="n">
         <f aca="false">$B$19*H11</f>
-        <v>57.03364764864</v>
+        <v>28.51682382432</v>
       </c>
       <c r="I19" s="35" t="n">
         <f aca="false">$B$19*I11</f>
@@ -1801,7 +1765,7 @@
       </c>
       <c r="J19" s="35" t="n">
         <f aca="false">SUM(E19:I19)</f>
-        <v>293.391091082253</v>
+        <v>264.874267257933</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,23 +1783,23 @@
       </c>
       <c r="F20" s="35" t="n">
         <f aca="false">F12*$D$20</f>
-        <v>224.8238916</v>
+        <v>227.09484</v>
       </c>
       <c r="G20" s="35" t="n">
         <f aca="false">G12*$D$20</f>
-        <v>687.961108296</v>
+        <v>694.9102104</v>
       </c>
       <c r="H20" s="35" t="n">
         <f aca="false">H12*$D$20</f>
-        <v>231.567709052434</v>
+        <v>472.538943072</v>
       </c>
       <c r="I20" s="35" t="n">
         <f aca="false">I12*$D$20</f>
-        <v>236.199063233482</v>
+        <v>481.98972193344</v>
       </c>
       <c r="J20" s="35" t="n">
         <f aca="false">SUM(E20:I20)</f>
-        <v>2048.47777218192</v>
+        <v>2544.45971540544</v>
       </c>
       <c r="K20" s="55"/>
     </row>
@@ -1852,23 +1816,23 @@
       </c>
       <c r="F21" s="56" t="n">
         <f aca="false">SUM(F17:F20)</f>
-        <v>1656.45553632</v>
+        <v>1658.72648472</v>
       </c>
       <c r="G21" s="56" t="n">
         <f aca="false">SUM(G17:G20)</f>
-        <v>2134.2465507024</v>
+        <v>2141.1956528064</v>
       </c>
       <c r="H21" s="56" t="n">
         <f aca="false">SUM(H17:H20)</f>
-        <v>1706.77886030696</v>
+        <v>1919.23327050221</v>
       </c>
       <c r="I21" s="56" t="n">
         <f aca="false">SUM(I17:I20)</f>
-        <v>1740.9144375131</v>
+        <v>1986.70509621306</v>
       </c>
       <c r="J21" s="56" t="n">
         <f aca="false">SUM(J17:J20)</f>
-        <v>9296.44580084246</v>
+        <v>9763.91092024166</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,27 +1856,27 @@
       <c r="D23" s="47"/>
       <c r="E23" s="48" t="n">
         <f aca="false">E15+E21</f>
-        <v>51788.690416</v>
+        <v>51288.690416</v>
       </c>
       <c r="F23" s="48" t="n">
         <f aca="false">F15+F21</f>
-        <v>50772.25033632</v>
+        <v>50292.97928472</v>
       </c>
       <c r="G23" s="48" t="n">
         <f aca="false">G15+G21</f>
-        <v>53786.9229267024</v>
+        <v>53360.7535088064</v>
       </c>
       <c r="H23" s="48" t="n">
         <f aca="false">H15+H21</f>
-        <v>48500.871904059</v>
+        <v>42649.0754836222</v>
       </c>
       <c r="I23" s="48" t="n">
         <f aca="false">I15+I21</f>
-        <v>49470.8893421401</v>
+        <v>52255.5473631955</v>
       </c>
       <c r="J23" s="48" t="n">
         <f aca="false">J15+J21</f>
-        <v>254319.624925221</v>
+        <v>249847.046056344</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2496,96 +2460,100 @@
       </c>
       <c r="K44" s="55"/>
     </row>
-    <row r="45" s="92" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="86" t="s">
+    <row r="45" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="87" t="n">
+      <c r="B45" s="32" t="n">
         <v>1740</v>
       </c>
-      <c r="C45" s="88"/>
-      <c r="D45" s="89" t="n">
+      <c r="C45" s="26"/>
+      <c r="D45" s="66" t="n">
         <v>8</v>
       </c>
-      <c r="E45" s="90" t="n">
+      <c r="E45" s="67" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="F45" s="90" t="n">
+      <c r="F45" s="67" t="n">
         <f aca="false">B45*D45</f>
         <v>13920</v>
       </c>
-      <c r="G45" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" s="91" t="n">
+      <c r="G45" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="35" t="n">
         <f aca="false">SUM(E45:I45)</f>
         <v>13920</v>
       </c>
     </row>
-    <row r="46" s="92" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="86" t="s">
+    <row r="46" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="88" t="n">
+      <c r="B46" s="26" t="n">
         <v>500</v>
       </c>
-      <c r="C46" s="93" t="n">
+      <c r="C46" s="73" t="n">
         <v>4</v>
       </c>
-      <c r="D46" s="93"/>
-      <c r="E46" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="90" t="n">
+      <c r="D46" s="73"/>
+      <c r="E46" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="67" t="n">
         <v>2000</v>
       </c>
-      <c r="H46" s="90" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="90" t="n">
+      <c r="H46" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="67" t="n">
         <v>0</v>
       </c>
       <c r="J46" s="43" t="n">
         <f aca="false">SUM(E46:I46)</f>
         <v>2000</v>
       </c>
-      <c r="K46" s="94"/>
-    </row>
-    <row r="47" s="92" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="86" t="s">
+      <c r="K46" s="55"/>
+    </row>
+    <row r="47" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="88" t="n">
+      <c r="B47" s="26" t="n">
         <v>1000</v>
       </c>
-      <c r="C47" s="93"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="90"/>
-      <c r="F47" s="90"/>
-      <c r="G47" s="95" t="n">
+      <c r="C47" s="73"/>
+      <c r="D47" s="73"/>
+      <c r="E47" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" s="86" t="n">
         <v>1000</v>
       </c>
-      <c r="H47" s="95" t="n">
+      <c r="H47" s="86" t="n">
         <v>1000</v>
       </c>
-      <c r="I47" s="95" t="n">
+      <c r="I47" s="86" t="n">
         <v>1000</v>
       </c>
-      <c r="J47" s="91" t="n">
+      <c r="J47" s="35" t="n">
         <f aca="false">SUM(E47:I47)</f>
         <v>3000</v>
       </c>
-      <c r="K47" s="94"/>
+      <c r="K47" s="55"/>
     </row>
     <row r="48" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="27" t="s">
@@ -2603,15 +2571,15 @@
       <c r="E48" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="F48" s="90" t="n">
+      <c r="F48" s="67" t="n">
         <f aca="false">B48</f>
         <v>2500</v>
       </c>
-      <c r="G48" s="90" t="n">
+      <c r="G48" s="67" t="n">
         <f aca="false">B48</f>
         <v>2500</v>
       </c>
-      <c r="H48" s="95" t="n">
+      <c r="H48" s="86" t="n">
         <v>1000</v>
       </c>
       <c r="I48" s="67" t="n">
@@ -2731,10 +2699,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="96"/>
-      <c r="B52" s="97"/>
-      <c r="C52" s="97"/>
-      <c r="D52" s="98"/>
+      <c r="A52" s="87"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="88"/>
+      <c r="D52" s="89"/>
       <c r="E52" s="67"/>
       <c r="F52" s="67"/>
       <c r="G52" s="67"/>
@@ -2743,12 +2711,12 @@
       <c r="J52" s="67"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="99" t="s">
+      <c r="A53" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="B53" s="100"/>
-      <c r="C53" s="100"/>
-      <c r="D53" s="101"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="92"/>
       <c r="E53" s="48" t="n">
         <f aca="false">E28+E37+E51</f>
         <v>64492</v>
@@ -2773,155 +2741,155 @@
         <f aca="false">J28+J37+J51</f>
         <v>129340.20029152</v>
       </c>
-      <c r="K53" s="102"/>
+      <c r="K53" s="93"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="103"/>
-      <c r="B54" s="104"/>
-      <c r="C54" s="104"/>
-      <c r="D54" s="105"/>
-      <c r="E54" s="106"/>
-      <c r="F54" s="106"/>
-      <c r="G54" s="106"/>
-      <c r="H54" s="106"/>
-      <c r="I54" s="106"/>
+      <c r="A54" s="94"/>
+      <c r="B54" s="95"/>
+      <c r="C54" s="95"/>
+      <c r="D54" s="96"/>
+      <c r="E54" s="97"/>
+      <c r="F54" s="97"/>
+      <c r="G54" s="97"/>
+      <c r="H54" s="97"/>
+      <c r="I54" s="97"/>
       <c r="J54" s="59"/>
-      <c r="K54" s="102"/>
+      <c r="K54" s="93"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="99" t="s">
+      <c r="A55" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="100"/>
-      <c r="C55" s="100"/>
-      <c r="D55" s="101"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="92"/>
       <c r="E55" s="48" t="n">
         <f aca="false">E23+E53</f>
-        <v>116280.690416</v>
+        <v>115780.690416</v>
       </c>
       <c r="F55" s="48" t="n">
         <f aca="false">F23+F53</f>
-        <v>76377.49033632</v>
+        <v>75898.21928472</v>
       </c>
       <c r="G55" s="48" t="n">
         <f aca="false">G23+G53</f>
-        <v>73157.5317267024</v>
+        <v>72731.3623088064</v>
       </c>
       <c r="H55" s="48" t="n">
         <f aca="false">H23+H53</f>
-        <v>61059.348880059</v>
+        <v>55207.5524596222</v>
       </c>
       <c r="I55" s="48" t="n">
         <f aca="false">I23+I53</f>
-        <v>56784.7638576601</v>
+        <v>59569.4218787155</v>
       </c>
       <c r="J55" s="56" t="n">
         <f aca="false">SUM(E55:I55)</f>
-        <v>383659.825216742</v>
-      </c>
-      <c r="K55" s="102"/>
+        <v>379187.246347864</v>
+      </c>
+      <c r="K55" s="93"/>
     </row>
     <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="103"/>
-      <c r="B56" s="107" t="s">
+      <c r="A56" s="94"/>
+      <c r="B56" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="C56" s="107" t="s">
+      <c r="C56" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="D56" s="105"/>
-      <c r="E56" s="106"/>
-      <c r="F56" s="106"/>
-      <c r="G56" s="106"/>
-      <c r="H56" s="106"/>
-      <c r="I56" s="106"/>
+      <c r="D56" s="96"/>
+      <c r="E56" s="97"/>
+      <c r="F56" s="97"/>
+      <c r="G56" s="97"/>
+      <c r="H56" s="97"/>
+      <c r="I56" s="97"/>
       <c r="J56" s="59"/>
-      <c r="K56" s="102"/>
+      <c r="K56" s="93"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="99" t="s">
+      <c r="A57" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="B57" s="108" t="n">
+      <c r="B57" s="99" t="n">
         <v>0.557</v>
       </c>
-      <c r="C57" s="109" t="s">
+      <c r="C57" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="D57" s="101"/>
+      <c r="D57" s="92"/>
       <c r="E57" s="48" t="n">
         <f aca="false">E15*0.557</f>
-        <v>27699.96648</v>
+        <v>27421.46648</v>
       </c>
       <c r="F57" s="48" t="n">
         <f aca="false">F15*0.557</f>
-        <v>27357.4977036</v>
+        <v>27089.2788096</v>
       </c>
       <c r="G57" s="48" t="n">
         <f aca="false">G15*0.557</f>
-        <v>28770.540741432</v>
+        <v>28529.293725792</v>
       </c>
       <c r="H57" s="48" t="n">
         <f aca="false">H15*0.557</f>
-        <v>26064.3098253699</v>
+        <v>22686.5221127078</v>
       </c>
       <c r="I57" s="48" t="n">
         <f aca="false">I15*0.557</f>
-        <v>26585.5960218773</v>
+        <v>27999.7451427092</v>
       </c>
       <c r="J57" s="56" t="n">
         <f aca="false">SUM(E57:I57)</f>
-        <v>136477.910772279</v>
+        <v>133726.306270809</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="103"/>
-      <c r="B58" s="110"/>
-      <c r="C58" s="104"/>
-      <c r="D58" s="105"/>
-      <c r="E58" s="106"/>
-      <c r="F58" s="106"/>
-      <c r="G58" s="106"/>
-      <c r="H58" s="106"/>
-      <c r="I58" s="106"/>
+      <c r="A58" s="94"/>
+      <c r="B58" s="101"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="96"/>
+      <c r="E58" s="97"/>
+      <c r="F58" s="97"/>
+      <c r="G58" s="97"/>
+      <c r="H58" s="97"/>
+      <c r="I58" s="97"/>
       <c r="J58" s="59"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="111" t="s">
+      <c r="A59" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="B59" s="112"/>
-      <c r="C59" s="112"/>
-      <c r="D59" s="113"/>
-      <c r="E59" s="114" t="n">
+      <c r="B59" s="103"/>
+      <c r="C59" s="103"/>
+      <c r="D59" s="104"/>
+      <c r="E59" s="105" t="n">
         <f aca="false">E55+E57</f>
-        <v>143980.656896</v>
-      </c>
-      <c r="F59" s="114" t="n">
+        <v>143202.156896</v>
+      </c>
+      <c r="F59" s="105" t="n">
         <f aca="false">F55+F57</f>
-        <v>103734.98803992</v>
-      </c>
-      <c r="G59" s="114" t="n">
+        <v>102987.49809432</v>
+      </c>
+      <c r="G59" s="105" t="n">
         <f aca="false">G55+G57</f>
-        <v>101928.072468134</v>
-      </c>
-      <c r="H59" s="114" t="n">
+        <v>101260.656034598</v>
+      </c>
+      <c r="H59" s="105" t="n">
         <f aca="false">H55+H57</f>
-        <v>87123.6587054288</v>
-      </c>
-      <c r="I59" s="114" t="n">
+        <v>77894.0745723301</v>
+      </c>
+      <c r="I59" s="105" t="n">
         <f aca="false">I55+I57</f>
-        <v>83370.3598795374</v>
-      </c>
-      <c r="J59" s="114" t="n">
+        <v>87569.1670214247</v>
+      </c>
+      <c r="J59" s="105" t="n">
         <f aca="false">J55+J57</f>
-        <v>520137.735989021</v>
-      </c>
-      <c r="K59" s="102"/>
+        <v>512913.552618673</v>
+      </c>
+      <c r="K59" s="93"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="115"/>
-      <c r="D60" s="116"/>
+      <c r="A60" s="106"/>
+      <c r="D60" s="107"/>
       <c r="E60" s="55"/>
       <c r="F60" s="55"/>
       <c r="G60" s="55"/>
@@ -2930,8 +2898,8 @@
       <c r="J60" s="55"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="117"/>
-      <c r="D61" s="116"/>
+      <c r="A61" s="108"/>
+      <c r="D61" s="107"/>
       <c r="E61" s="55"/>
       <c r="F61" s="55"/>
       <c r="G61" s="55"/>
@@ -4184,31 +4152,31 @@
       <c r="K44" s="55"/>
     </row>
     <row r="45" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="118" t="s">
+      <c r="A45" s="109" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="119" t="n">
+      <c r="B45" s="110" t="n">
         <v>1740</v>
       </c>
-      <c r="C45" s="120"/>
-      <c r="D45" s="121" t="n">
+      <c r="C45" s="111"/>
+      <c r="D45" s="112" t="n">
         <v>8</v>
       </c>
-      <c r="E45" s="95" t="n">
+      <c r="E45" s="86" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="F45" s="95" t="n">
+      <c r="F45" s="86" t="n">
         <f aca="false">B45*D45</f>
         <v>13920</v>
       </c>
-      <c r="G45" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" s="95" t="n">
+      <c r="G45" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="86" t="n">
         <v>0</v>
       </c>
       <c r="J45" s="43" t="n">
@@ -4217,32 +4185,32 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="118" t="s">
+      <c r="A46" s="109" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="120" t="n">
+      <c r="B46" s="111" t="n">
         <v>500</v>
       </c>
-      <c r="C46" s="122" t="n">
+      <c r="C46" s="113" t="n">
         <v>4</v>
       </c>
-      <c r="D46" s="122"/>
-      <c r="E46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="95" t="n">
+      <c r="D46" s="113"/>
+      <c r="E46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="86" t="n">
         <v>2000</v>
       </c>
-      <c r="H46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" s="95" t="n">
+      <c r="H46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="86" t="n">
         <v>0</v>
       </c>
       <c r="K46" s="55"/>
@@ -4263,11 +4231,11 @@
       <c r="E47" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="F47" s="95" t="n">
+      <c r="F47" s="86" t="n">
         <f aca="false">B47</f>
         <v>2500</v>
       </c>
-      <c r="G47" s="95" t="n">
+      <c r="G47" s="86" t="n">
         <f aca="false">B47</f>
         <v>2500</v>
       </c>
@@ -4391,10 +4359,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="96"/>
-      <c r="B51" s="97"/>
-      <c r="C51" s="97"/>
-      <c r="D51" s="98"/>
+      <c r="A51" s="87"/>
+      <c r="B51" s="88"/>
+      <c r="C51" s="88"/>
+      <c r="D51" s="89"/>
       <c r="E51" s="67"/>
       <c r="F51" s="67"/>
       <c r="G51" s="67"/>
@@ -4403,12 +4371,12 @@
       <c r="J51" s="67"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="99" t="s">
+      <c r="A52" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="100"/>
-      <c r="C52" s="100"/>
-      <c r="D52" s="101"/>
+      <c r="B52" s="91"/>
+      <c r="C52" s="91"/>
+      <c r="D52" s="92"/>
       <c r="E52" s="48" t="n">
         <f aca="false">E28+E37+E50</f>
         <v>104492</v>
@@ -4433,28 +4401,28 @@
         <f aca="false">J28+J37+J50</f>
         <v>177260.20029152</v>
       </c>
-      <c r="K52" s="102"/>
+      <c r="K52" s="93"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="103"/>
-      <c r="B53" s="104"/>
-      <c r="C53" s="104"/>
-      <c r="D53" s="105"/>
-      <c r="E53" s="106"/>
-      <c r="F53" s="106"/>
-      <c r="G53" s="106"/>
-      <c r="H53" s="106"/>
-      <c r="I53" s="106"/>
+      <c r="A53" s="94"/>
+      <c r="B53" s="95"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="96"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+      <c r="I53" s="97"/>
       <c r="J53" s="59"/>
-      <c r="K53" s="102"/>
+      <c r="K53" s="93"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="99" t="s">
+      <c r="A54" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="100"/>
-      <c r="C54" s="100"/>
-      <c r="D54" s="101"/>
+      <c r="B54" s="91"/>
+      <c r="C54" s="91"/>
+      <c r="D54" s="92"/>
       <c r="E54" s="48" t="n">
         <f aca="false">E23+E52</f>
         <v>151530.690416</v>
@@ -4479,36 +4447,36 @@
         <f aca="false">SUM(E54:I54)</f>
         <v>394940.634456742</v>
       </c>
-      <c r="K54" s="102"/>
+      <c r="K54" s="93"/>
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="103"/>
-      <c r="B55" s="107" t="s">
+      <c r="A55" s="94"/>
+      <c r="B55" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="107" t="s">
+      <c r="C55" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="105"/>
-      <c r="E55" s="106"/>
-      <c r="F55" s="106"/>
-      <c r="G55" s="106"/>
-      <c r="H55" s="106"/>
-      <c r="I55" s="106"/>
+      <c r="D55" s="96"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
+      <c r="H55" s="97"/>
+      <c r="I55" s="97"/>
       <c r="J55" s="59"/>
-      <c r="K55" s="102"/>
+      <c r="K55" s="93"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="99" t="s">
+      <c r="A56" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="B56" s="108" t="n">
+      <c r="B56" s="99" t="n">
         <v>0.557</v>
       </c>
-      <c r="C56" s="109" t="s">
+      <c r="C56" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="101"/>
+      <c r="D56" s="92"/>
       <c r="E56" s="48" t="n">
         <f aca="false">E15*0.557</f>
         <v>25054.21648</v>
@@ -4535,53 +4503,53 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="103"/>
-      <c r="B57" s="110"/>
-      <c r="C57" s="104"/>
-      <c r="D57" s="105"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="106"/>
-      <c r="G57" s="106"/>
-      <c r="H57" s="106"/>
-      <c r="I57" s="106"/>
+      <c r="A57" s="94"/>
+      <c r="B57" s="101"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="96"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="97"/>
+      <c r="G57" s="97"/>
+      <c r="H57" s="97"/>
+      <c r="I57" s="97"/>
       <c r="J57" s="59"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="111" t="s">
+      <c r="A58" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="112"/>
-      <c r="C58" s="112"/>
-      <c r="D58" s="113"/>
-      <c r="E58" s="114" t="n">
+      <c r="B58" s="103"/>
+      <c r="C58" s="103"/>
+      <c r="D58" s="104"/>
+      <c r="E58" s="105" t="n">
         <f aca="false">E54+E56</f>
         <v>176584.906896</v>
       </c>
-      <c r="F58" s="114" t="n">
+      <c r="F58" s="105" t="n">
         <f aca="false">F54+F56</f>
         <v>96191.32303992</v>
       </c>
-      <c r="G58" s="114" t="n">
+      <c r="G58" s="105" t="n">
         <f aca="false">G54+G56</f>
         <v>93233.5341681344</v>
       </c>
-      <c r="H58" s="114" t="n">
+      <c r="H58" s="105" t="n">
         <f aca="false">H54+H56</f>
         <v>77275.2296394288</v>
       </c>
-      <c r="I58" s="114" t="n">
+      <c r="I58" s="105" t="n">
         <f aca="false">I54+I56</f>
         <v>74364.9622322174</v>
       </c>
-      <c r="J58" s="114" t="n">
+      <c r="J58" s="105" t="n">
         <f aca="false">J54+J56</f>
         <v>517649.955975701</v>
       </c>
-      <c r="K58" s="102"/>
+      <c r="K58" s="93"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="115"/>
-      <c r="D59" s="116"/>
+      <c r="A59" s="106"/>
+      <c r="D59" s="107"/>
       <c r="E59" s="55"/>
       <c r="F59" s="55"/>
       <c r="G59" s="55"/>
@@ -4590,8 +4558,8 @@
       <c r="J59" s="55"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="117"/>
-      <c r="D60" s="116"/>
+      <c r="A60" s="108"/>
+      <c r="D60" s="107"/>
       <c r="E60" s="55"/>
       <c r="F60" s="55"/>
       <c r="G60" s="55"/>
@@ -5358,32 +5326,32 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="28" s="123" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="118" t="s">
+    <row r="28" s="114" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="109" t="s">
         <v>86</v>
       </c>
-      <c r="B28" s="119" t="n">
+      <c r="B28" s="110" t="n">
         <v>1740</v>
       </c>
-      <c r="C28" s="120"/>
-      <c r="D28" s="121" t="n">
+      <c r="C28" s="111"/>
+      <c r="D28" s="112" t="n">
         <v>8</v>
       </c>
-      <c r="E28" s="95" t="n">
+      <c r="E28" s="86" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>
-      <c r="F28" s="95" t="n">
+      <c r="F28" s="86" t="n">
         <f aca="false">B28*D28</f>
         <v>13920</v>
       </c>
-      <c r="G28" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="I28" s="95" t="n">
+      <c r="G28" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="86" t="n">
         <v>0</v>
       </c>
       <c r="J28" s="43" t="n">
@@ -5876,36 +5844,36 @@
       </c>
       <c r="K45" s="55"/>
     </row>
-    <row r="46" s="123" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="118" t="s">
+    <row r="46" s="114" customFormat="true" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="109" t="s">
         <v>73</v>
       </c>
-      <c r="B46" s="120" t="n">
+      <c r="B46" s="111" t="n">
         <v>500</v>
       </c>
-      <c r="C46" s="122" t="n">
+      <c r="C46" s="113" t="n">
         <v>4</v>
       </c>
-      <c r="D46" s="122"/>
-      <c r="E46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="G46" s="95" t="n">
+      <c r="D46" s="113"/>
+      <c r="E46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" s="86" t="n">
         <v>2000</v>
       </c>
-      <c r="H46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="I46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" s="95" t="n">
-        <v>0</v>
-      </c>
-      <c r="K46" s="124"/>
+      <c r="H46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="86" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="115"/>
     </row>
     <row r="47" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="27" t="s">
@@ -5923,11 +5891,11 @@
       <c r="E47" s="67" t="n">
         <v>0</v>
       </c>
-      <c r="F47" s="95" t="n">
+      <c r="F47" s="86" t="n">
         <f aca="false">B47</f>
         <v>2500</v>
       </c>
-      <c r="G47" s="95" t="n">
+      <c r="G47" s="86" t="n">
         <f aca="false">B47</f>
         <v>2500</v>
       </c>
@@ -6046,10 +6014,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="96"/>
-      <c r="B51" s="97"/>
-      <c r="C51" s="97"/>
-      <c r="D51" s="98"/>
+      <c r="A51" s="87"/>
+      <c r="B51" s="88"/>
+      <c r="C51" s="88"/>
+      <c r="D51" s="89"/>
       <c r="E51" s="67"/>
       <c r="F51" s="67"/>
       <c r="G51" s="67"/>
@@ -6058,12 +6026,12 @@
       <c r="J51" s="67"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="99" t="s">
+      <c r="A52" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="B52" s="100"/>
-      <c r="C52" s="100"/>
-      <c r="D52" s="101"/>
+      <c r="B52" s="91"/>
+      <c r="C52" s="91"/>
+      <c r="D52" s="92"/>
       <c r="E52" s="48" t="n">
         <f aca="false">E29+E38+E50</f>
         <v>104442</v>
@@ -6088,28 +6056,28 @@
         <f aca="false">J29+J38+J50</f>
         <v>161841.2552</v>
       </c>
-      <c r="K52" s="102"/>
+      <c r="K52" s="93"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="103"/>
-      <c r="B53" s="104"/>
-      <c r="C53" s="104"/>
-      <c r="D53" s="105"/>
-      <c r="E53" s="106"/>
-      <c r="F53" s="106"/>
-      <c r="G53" s="106"/>
-      <c r="H53" s="106"/>
-      <c r="I53" s="106"/>
+      <c r="A53" s="94"/>
+      <c r="B53" s="95"/>
+      <c r="C53" s="95"/>
+      <c r="D53" s="96"/>
+      <c r="E53" s="97"/>
+      <c r="F53" s="97"/>
+      <c r="G53" s="97"/>
+      <c r="H53" s="97"/>
+      <c r="I53" s="97"/>
       <c r="J53" s="59"/>
-      <c r="K53" s="102"/>
+      <c r="K53" s="93"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="99" t="s">
+      <c r="A54" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="100"/>
-      <c r="C54" s="100"/>
-      <c r="D54" s="101"/>
+      <c r="B54" s="91"/>
+      <c r="C54" s="91"/>
+      <c r="D54" s="92"/>
       <c r="E54" s="48" t="n">
         <f aca="false">E23+E52</f>
         <v>151480.690416</v>
@@ -6134,36 +6102,36 @@
         <f aca="false">SUM(E54:I54)</f>
         <v>393441.689365222</v>
       </c>
-      <c r="K54" s="102"/>
+      <c r="K54" s="93"/>
     </row>
     <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="103"/>
-      <c r="B55" s="107" t="s">
+      <c r="A55" s="94"/>
+      <c r="B55" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="C55" s="107" t="s">
+      <c r="C55" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="D55" s="105"/>
-      <c r="E55" s="106"/>
-      <c r="F55" s="106"/>
-      <c r="G55" s="106"/>
-      <c r="H55" s="106"/>
-      <c r="I55" s="106"/>
+      <c r="D55" s="96"/>
+      <c r="E55" s="97"/>
+      <c r="F55" s="97"/>
+      <c r="G55" s="97"/>
+      <c r="H55" s="97"/>
+      <c r="I55" s="97"/>
       <c r="J55" s="59"/>
-      <c r="K55" s="102"/>
+      <c r="K55" s="93"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="99" t="s">
+      <c r="A56" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="B56" s="108" t="n">
+      <c r="B56" s="99" t="n">
         <v>0.557</v>
       </c>
-      <c r="C56" s="109" t="s">
+      <c r="C56" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="101"/>
+      <c r="D56" s="92"/>
       <c r="E56" s="48" t="n">
         <f aca="false">E15*0.557</f>
         <v>25054.21648</v>
@@ -6190,53 +6158,53 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="103"/>
-      <c r="B57" s="110"/>
-      <c r="C57" s="104"/>
-      <c r="D57" s="105"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="106"/>
-      <c r="G57" s="106"/>
-      <c r="H57" s="106"/>
-      <c r="I57" s="106"/>
+      <c r="A57" s="94"/>
+      <c r="B57" s="101"/>
+      <c r="C57" s="95"/>
+      <c r="D57" s="96"/>
+      <c r="E57" s="97"/>
+      <c r="F57" s="97"/>
+      <c r="G57" s="97"/>
+      <c r="H57" s="97"/>
+      <c r="I57" s="97"/>
       <c r="J57" s="59"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="111" t="s">
+      <c r="A58" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="B58" s="112"/>
-      <c r="C58" s="112"/>
-      <c r="D58" s="113"/>
-      <c r="E58" s="114" t="n">
+      <c r="B58" s="103"/>
+      <c r="C58" s="103"/>
+      <c r="D58" s="104"/>
+      <c r="E58" s="105" t="n">
         <f aca="false">E54+E56</f>
         <v>176534.906896</v>
       </c>
-      <c r="F58" s="114" t="n">
+      <c r="F58" s="105" t="n">
         <f aca="false">F54+F56</f>
         <v>96018.08303992</v>
       </c>
-      <c r="G58" s="114" t="n">
+      <c r="G58" s="105" t="n">
         <f aca="false">G54+G56</f>
         <v>92762.9253681344</v>
       </c>
-      <c r="H58" s="114" t="n">
+      <c r="H58" s="105" t="n">
         <f aca="false">H54+H56</f>
         <v>76795.7126634288</v>
       </c>
-      <c r="I58" s="114" t="n">
+      <c r="I58" s="105" t="n">
         <f aca="false">I54+I56</f>
         <v>74039.3829166974</v>
       </c>
-      <c r="J58" s="114" t="n">
+      <c r="J58" s="105" t="n">
         <f aca="false">J54+J56</f>
         <v>516151.010884181</v>
       </c>
-      <c r="K58" s="102"/>
+      <c r="K58" s="93"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="115"/>
-      <c r="D59" s="116"/>
+      <c r="A59" s="106"/>
+      <c r="D59" s="107"/>
       <c r="E59" s="55"/>
       <c r="F59" s="55"/>
       <c r="G59" s="55"/>
@@ -6245,8 +6213,8 @@
       <c r="J59" s="55"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="117"/>
-      <c r="D60" s="116"/>
+      <c r="A60" s="108"/>
+      <c r="D60" s="107"/>
       <c r="E60" s="55"/>
       <c r="F60" s="55"/>
       <c r="G60" s="55"/>
@@ -6282,59 +6250,59 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="116" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
+      <c r="B1" s="117"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="127"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
-      <c r="E2" s="127"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="128" t="s">
+      <c r="A3" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="119" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="128" t="s">
+      <c r="C3" s="119" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="128" t="s">
+      <c r="D3" s="119" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="128" t="s">
+      <c r="E3" s="119" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="118" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="117" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="127" t="n">
+      <c r="C4" s="118" t="n">
         <v>1</v>
       </c>
-      <c r="D4" s="127" t="n">
+      <c r="D4" s="118" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="127" t="n">
+      <c r="E4" s="118" t="n">
         <f aca="false">C4*D4</f>
         <v>2</v>
       </c>

</xml_diff>